<commit_message>
Added more results to the Classification Rates excel file.  Also added varaible importance plot code to H1B_code file.
</commit_message>
<xml_diff>
--- a/Project_2/Classification Rates RF and J48.xlsx
+++ b/Project_2/Classification Rates RF and J48.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>H1B_1</t>
   </si>
@@ -91,13 +91,70 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>GBM - No Wage Conversion</t>
+  </si>
+  <si>
+    <t>Trials</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>File 1</t>
+  </si>
+  <si>
+    <t>File 2</t>
+  </si>
+  <si>
+    <t>File 3</t>
+  </si>
+  <si>
+    <t>File 4</t>
+  </si>
+  <si>
+    <t>File 5</t>
+  </si>
+  <si>
+    <t>File 6</t>
+  </si>
+  <si>
+    <t>File 7</t>
+  </si>
+  <si>
+    <t>File 8</t>
+  </si>
+  <si>
+    <t>File 9</t>
+  </si>
+  <si>
+    <t>File 10</t>
+  </si>
+  <si>
+    <t>Std Dev.</t>
+  </si>
+  <si>
+    <t>University of Texas Arlington Results for J48:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +175,20 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -133,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -141,30 +212,246 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,247 +744,530 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="19"/>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="22">
         <f>1-0.2262</f>
         <v>0.77380000000000004</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="23">
         <f>1-0.2255</f>
         <v>0.77449999999999997</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="23">
         <v>0.86336900000000005</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="23">
         <v>0.86125399999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="24">
+        <v>0.73202780000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="15">
         <f>1-0.2299</f>
         <v>0.77010000000000001</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <f>1-0.2266</f>
         <v>0.77339999999999998</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>0.85167999999999999</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>0.85397800000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="7">
+        <v>0.72816119999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="15">
         <f>1-0.2326</f>
         <v>0.76739999999999997</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <f>1-0.2277</f>
         <v>0.77229999999999999</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>0.85154099999999999</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>0.85236599999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" s="7">
+        <v>0.72744520000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="15">
         <f>1-0.228</f>
         <v>0.77200000000000002</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <f>1-0.2279</f>
         <v>0.77210000000000001</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>0.85602199999999995</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="8">
         <v>0.85731199999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" s="7">
+        <v>0.72973650000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="15">
         <f>1-0.2309</f>
         <v>0.76910000000000001</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <f>1-0.2265</f>
         <v>0.77349999999999997</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="8">
         <v>0.86100399999999999</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="8">
         <v>0.85856600000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" s="7">
+        <v>0.72866249999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="15">
         <f>1-0.2265</f>
         <v>0.77349999999999997</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <f>1-0.2285</f>
         <v>0.77149999999999996</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="8">
         <v>0.85362000000000005</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="8">
         <v>0.85426500000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8" s="7">
+        <v>0.72801800000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="15">
         <f>1-0.2285</f>
         <v>0.77149999999999996</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <f>1-0.2279</f>
         <v>0.77210000000000001</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="8">
         <v>0.85021000000000002</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="8">
         <v>0.85038899999999995</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9" s="7">
+        <v>0.72962910000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="15">
         <f>1-0.2314</f>
         <v>0.76859999999999995</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <f>1-0.2307</f>
         <v>0.76929999999999998</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="8">
         <v>0.85401400000000005</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="8">
         <v>0.85670299999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="F10" s="7">
+        <v>0.73055990000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="15">
         <f>1-0.2314</f>
         <v>0.76859999999999995</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <f>1-0.2291</f>
         <v>0.77090000000000003</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="8">
         <v>0.84989199999999998</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="8">
         <v>0.84992800000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11" s="7">
+        <v>0.72812540000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="16">
         <f>1-0.2282</f>
         <v>0.77180000000000004</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="12">
         <f>1-0.2269</f>
         <v>0.77310000000000001</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="13">
         <v>0.85791600000000001</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="13">
         <v>0.85433199999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F12" s="14">
+        <v>0.7284119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="17">
         <f>AVERAGE(B3:B12)</f>
         <v>0.77063999999999999</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="10">
         <f t="shared" ref="C13:E13" si="0">AVERAGE(C3:C12)</f>
         <v>0.77227000000000001</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="10">
         <f t="shared" si="0"/>
         <v>0.85492679999999999</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="10">
         <f t="shared" si="0"/>
         <v>0.85490929999999987</v>
       </c>
+      <c r="F13" s="10">
+        <f>AVERAGE(F3:F12)</f>
+        <v>0.72907775000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="28">
+        <v>68.642700000000005</v>
+      </c>
+      <c r="C20" s="9">
+        <v>59.187100000000001</v>
+      </c>
+      <c r="D20" s="9">
+        <v>68.886499999999998</v>
+      </c>
+      <c r="E20" s="9">
+        <v>59.720700000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="27">
+        <v>68.811199999999999</v>
+      </c>
+      <c r="C21" s="4">
+        <v>60.608600000000003</v>
+      </c>
+      <c r="D21" s="4">
+        <v>69.011799999999994</v>
+      </c>
+      <c r="E21" s="4">
+        <v>60.759</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="27">
+        <v>68.758600000000001</v>
+      </c>
+      <c r="C22" s="4">
+        <v>60.082099999999997</v>
+      </c>
+      <c r="D22" s="4">
+        <v>68.474800000000002</v>
+      </c>
+      <c r="E22" s="4">
+        <v>60.741100000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="27">
+        <v>68.400499999999994</v>
+      </c>
+      <c r="C23" s="4">
+        <v>60.914000000000001</v>
+      </c>
+      <c r="D23" s="4">
+        <v>68.564300000000003</v>
+      </c>
+      <c r="E23" s="4">
+        <v>60.991799999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="27">
+        <v>68.347899999999996</v>
+      </c>
+      <c r="C24" s="4">
+        <v>59.597799999999999</v>
+      </c>
+      <c r="D24" s="4">
+        <v>68.403199999999998</v>
+      </c>
+      <c r="E24" s="4">
+        <v>60.150399999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="27">
+        <v>68.769099999999995</v>
+      </c>
+      <c r="C25" s="4">
+        <v>59.566200000000002</v>
+      </c>
+      <c r="D25" s="4">
+        <v>68.832800000000006</v>
+      </c>
+      <c r="E25" s="4">
+        <v>59.702800000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="27">
+        <v>69.685199999999995</v>
+      </c>
+      <c r="C26" s="4">
+        <v>60.871899999999997</v>
+      </c>
+      <c r="D26" s="4">
+        <v>68.886499999999998</v>
+      </c>
+      <c r="E26" s="4">
+        <v>60.4726</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="27">
+        <v>68.927000000000007</v>
+      </c>
+      <c r="C27" s="4">
+        <v>59.376600000000003</v>
+      </c>
+      <c r="D27" s="4">
+        <v>68.617999999999995</v>
+      </c>
+      <c r="E27" s="4">
+        <v>60.669499999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="27">
+        <v>68.853300000000004</v>
+      </c>
+      <c r="C28" s="4">
+        <v>60.3033</v>
+      </c>
+      <c r="D28" s="4">
+        <v>68.564300000000003</v>
+      </c>
+      <c r="E28" s="4">
+        <v>60.383099999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="32">
+        <v>68.537400000000005</v>
+      </c>
+      <c r="C29" s="11">
+        <v>60.334800000000001</v>
+      </c>
+      <c r="D29" s="11">
+        <v>68.761200000000002</v>
+      </c>
+      <c r="E29" s="11">
+        <v>60.562100000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="28">
+        <v>68.773290000000003</v>
+      </c>
+      <c r="C30" s="9">
+        <v>60.084240000000001</v>
+      </c>
+      <c r="D30" s="9">
+        <v>68.700339999999997</v>
+      </c>
+      <c r="E30" s="9">
+        <v>60.415309999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="27">
+        <v>0.13954507799999999</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.38947104300000002</v>
+      </c>
+      <c r="D31" s="4">
+        <v>4.1169125000000001E-2</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.189712557</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="27">
+        <v>0.37355732000000003</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.62407610000000002</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.20290169999999999</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.43556</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -715,7 +1285,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
+      <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -733,7 +1303,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2">
@@ -757,7 +1327,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3">
@@ -781,7 +1351,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4">
@@ -805,7 +1375,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B5">

</xml_diff>

<commit_message>
Finished running RF and J48 with the 80/20 and 66/34 splits
</commit_message>
<xml_diff>
--- a/Project_2/Classification Rates RF and J48.xlsx
+++ b/Project_2/Classification Rates RF and J48.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>H1B_1</t>
   </si>
@@ -36,18 +36,6 @@
     <t>Percent Correctly Classified</t>
   </si>
   <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>RF - wage converted to salary</t>
-  </si>
-  <si>
-    <t>J48</t>
-  </si>
-  <si>
-    <t>J48 - wage converted to salary</t>
-  </si>
-  <si>
     <t>H1B_2</t>
   </si>
   <si>
@@ -148,6 +136,30 @@
   </si>
   <si>
     <t>University of Texas Arlington Results for J48:</t>
+  </si>
+  <si>
+    <t>RF (80/20)</t>
+  </si>
+  <si>
+    <t>RF - wage converted to salary  (80/20)</t>
+  </si>
+  <si>
+    <t>J48 (80/20)</t>
+  </si>
+  <si>
+    <t>J48 - wage converted to salary (80/20)</t>
+  </si>
+  <si>
+    <t>RF (66/34)</t>
+  </si>
+  <si>
+    <t>RF - wage converted to salary  (66/34)</t>
+  </si>
+  <si>
+    <t>J48 (66/34)</t>
+  </si>
+  <si>
+    <t>J48 - wage converted to salary (66/34)</t>
   </si>
 </sst>
 </file>
@@ -204,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -393,12 +405,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -408,9 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -452,6 +485,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,339 +777,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="34.85546875" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="21">
+        <v>0.77939999999999998</v>
+      </c>
+      <c r="C3" s="22">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="D3" s="22">
+        <v>0.73850000000000005</v>
+      </c>
+      <c r="E3" s="22">
+        <v>0.77659999999999996</v>
+      </c>
+      <c r="F3" s="22">
+        <v>0.77110000000000001</v>
+      </c>
+      <c r="G3" s="22">
+        <v>0.77359999999999995</v>
+      </c>
+      <c r="H3" s="22">
+        <v>0.72870000000000001</v>
+      </c>
+      <c r="I3" s="22">
+        <v>0.7258</v>
+      </c>
+      <c r="J3" s="23">
+        <v>0.73202780000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="B4" s="14">
+        <v>0.76859999999999995</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.77459999999999996</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.73660000000000003</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.73673840000000002</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.72140000000000004</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.72816119999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="B5" s="14">
+        <v>0.77293909999999999</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.77149999999999996</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.72419999999999995</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.7671</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.76680000000000004</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.71368330000000002</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.71789999999999998</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.72744520000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="B6" s="14">
+        <v>0.76919999999999999</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.77059999999999995</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.74070000000000003</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.73480000000000001</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.76470000000000005</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.76480000000000004</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.70830000000000004</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.72973650000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="B7" s="14">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.78459999999999996</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.73821000000000003</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.7339</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.76790000000000003</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.71789999999999998</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.72040000000000004</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.72866249999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.77690000000000003</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.77829999999999999</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.7167</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.76690000000000003</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.7702</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.71630000000000005</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.72050000000000003</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.72801800000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0.77616490000000005</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.77710000000000001</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.7349</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.73240000000000005</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.76839550000000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.76649800000000001</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.70820159999999999</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.71532600000000002</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.72962910000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.76989249999999998</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.77275990000000006</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.72473120000000002</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.72419350000000005</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.76460050000000002</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.76871179999999995</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.71252369999999998</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.71389420000000003</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.73055990000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.7684588</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.77007170000000003</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.71899639999999998</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.71594979999999997</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.76460050000000002</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.76301920000000001</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.70303610000000005</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.70250900000000005</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.72812540000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.78315409999999996</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0.78225809999999996</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.72974910000000004</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0.74569890000000005</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.77566939999999995</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0.77440439999999999</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0.718638</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0.71779459999999995</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0.7284119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="16">
+        <f>AVERAGE(B3:B12)</f>
+        <v>0.77427094000000007</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" ref="C13:E13" si="0">AVERAGE(C3:C12)</f>
+        <v>0.77616896999999985</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.73008867</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.73436805999999999</v>
+      </c>
+      <c r="F13" s="9">
+        <f>AVERAGE(F3:F12)</f>
+        <v>0.76817659000000005</v>
+      </c>
+      <c r="G13" s="9">
+        <f>AVERAGE(G3:G12)</f>
+        <v>0.76948334000000007</v>
+      </c>
+      <c r="H13" s="9">
+        <f>AVERAGE(H3:H12)</f>
+        <v>0.71483827000000011</v>
+      </c>
+      <c r="I13" s="9">
+        <f>AVERAGE(I3:I12)</f>
+        <v>0.71654238000000015</v>
+      </c>
+      <c r="J13" s="9">
+        <f>AVERAGE(J3:J12)</f>
+        <v>0.72907775000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="30" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="22">
-        <f>1-0.2262</f>
-        <v>0.77380000000000004</v>
-      </c>
-      <c r="C3" s="23">
-        <f>1-0.2255</f>
-        <v>0.77449999999999997</v>
-      </c>
-      <c r="D3" s="23">
-        <v>0.86336900000000005</v>
-      </c>
-      <c r="E3" s="23">
-        <v>0.86125399999999996</v>
-      </c>
-      <c r="F3" s="24">
-        <v>0.73202780000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="15">
-        <f>1-0.2299</f>
-        <v>0.77010000000000001</v>
-      </c>
-      <c r="C4" s="6">
-        <f>1-0.2266</f>
-        <v>0.77339999999999998</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.85167999999999999</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.85397800000000001</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0.72816119999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="15">
-        <f>1-0.2326</f>
-        <v>0.76739999999999997</v>
-      </c>
-      <c r="C5" s="6">
-        <f>1-0.2277</f>
-        <v>0.77229999999999999</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.85154099999999999</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0.85236599999999996</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.72744520000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="15">
-        <f>1-0.228</f>
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="C6" s="6">
-        <f>1-0.2279</f>
-        <v>0.77210000000000001</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.85602199999999995</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.85731199999999996</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0.72973650000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="15">
-        <f>1-0.2309</f>
-        <v>0.76910000000000001</v>
-      </c>
-      <c r="C7" s="6">
-        <f>1-0.2265</f>
-        <v>0.77349999999999997</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.86100399999999999</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.85856600000000005</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0.72866249999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="15">
-        <f>1-0.2265</f>
-        <v>0.77349999999999997</v>
-      </c>
-      <c r="C8" s="6">
-        <f>1-0.2285</f>
-        <v>0.77149999999999996</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.85362000000000005</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0.85426500000000005</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0.72801800000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="15">
-        <f>1-0.2285</f>
-        <v>0.77149999999999996</v>
-      </c>
-      <c r="C9" s="6">
-        <f>1-0.2279</f>
-        <v>0.77210000000000001</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.85021000000000002</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.85038899999999995</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0.72962910000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="15">
-        <f>1-0.2314</f>
-        <v>0.76859999999999995</v>
-      </c>
-      <c r="C10" s="6">
-        <f>1-0.2307</f>
-        <v>0.76929999999999998</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.85401400000000005</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0.85670299999999999</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0.73055990000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="15">
-        <f>1-0.2314</f>
-        <v>0.76859999999999995</v>
-      </c>
-      <c r="C11" s="6">
-        <f>1-0.2291</f>
-        <v>0.77090000000000003</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.84989199999999998</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.84992800000000002</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0.72812540000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="16">
-        <f>1-0.2282</f>
-        <v>0.77180000000000004</v>
-      </c>
-      <c r="C12" s="12">
-        <f>1-0.2269</f>
-        <v>0.77310000000000001</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0.85791600000000001</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.85433199999999998</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0.7284119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="17">
-        <f>AVERAGE(B3:B12)</f>
-        <v>0.77063999999999999</v>
-      </c>
-      <c r="C13" s="10">
-        <f t="shared" ref="C13:E13" si="0">AVERAGE(C3:C12)</f>
-        <v>0.77227000000000001</v>
-      </c>
-      <c r="D13" s="10">
-        <f t="shared" si="0"/>
-        <v>0.85492679999999999</v>
-      </c>
-      <c r="E13" s="10">
-        <f t="shared" si="0"/>
-        <v>0.85490929999999987</v>
-      </c>
-      <c r="F13" s="10">
-        <f>AVERAGE(F3:F12)</f>
-        <v>0.72907775000000008</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="E19" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="31" t="s">
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="B20" s="27">
+        <v>68.642700000000005</v>
+      </c>
+      <c r="C20" s="8">
+        <v>59.187100000000001</v>
+      </c>
+      <c r="D20" s="8">
+        <v>68.886499999999998</v>
+      </c>
+      <c r="E20" s="8">
+        <v>59.720700000000001</v>
+      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="28">
-        <v>68.642700000000005</v>
-      </c>
-      <c r="C20" s="9">
-        <v>59.187100000000001</v>
-      </c>
-      <c r="D20" s="9">
-        <v>68.886499999999998</v>
-      </c>
-      <c r="E20" s="9">
-        <v>59.720700000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="27">
+      <c r="B21" s="26">
         <v>68.811199999999999</v>
       </c>
       <c r="C21" s="4">
@@ -1077,12 +1263,16 @@
       <c r="E21" s="4">
         <v>60.759</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="27">
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="26">
         <v>68.758600000000001</v>
       </c>
       <c r="C22" s="4">
@@ -1094,12 +1284,16 @@
       <c r="E22" s="4">
         <v>60.741100000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="27">
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="26">
         <v>68.400499999999994</v>
       </c>
       <c r="C23" s="4">
@@ -1111,12 +1305,16 @@
       <c r="E23" s="4">
         <v>60.991799999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="27">
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="26">
         <v>68.347899999999996</v>
       </c>
       <c r="C24" s="4">
@@ -1128,12 +1326,16 @@
       <c r="E24" s="4">
         <v>60.150399999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="27">
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="26">
         <v>68.769099999999995</v>
       </c>
       <c r="C25" s="4">
@@ -1145,12 +1347,16 @@
       <c r="E25" s="4">
         <v>59.702800000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="27">
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="26">
         <v>69.685199999999995</v>
       </c>
       <c r="C26" s="4">
@@ -1162,12 +1368,16 @@
       <c r="E26" s="4">
         <v>60.4726</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="27">
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="26">
         <v>68.927000000000007</v>
       </c>
       <c r="C27" s="4">
@@ -1179,12 +1389,16 @@
       <c r="E27" s="4">
         <v>60.669499999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="27">
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="26">
         <v>68.853300000000004</v>
       </c>
       <c r="C28" s="4">
@@ -1196,46 +1410,58 @@
       <c r="E28" s="4">
         <v>60.383099999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="32">
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="31">
         <v>68.537400000000005</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="10">
         <v>60.334800000000001</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="10">
         <v>68.761200000000002</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>60.562100000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="28">
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="27">
         <v>68.773290000000003</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <v>60.084240000000001</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="8">
         <v>68.700339999999997</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="8">
         <v>60.415309999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="27">
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="26">
         <v>0.13954507799999999</v>
       </c>
       <c r="C31" s="4">
@@ -1247,12 +1473,16 @@
       <c r="E31" s="4">
         <v>0.189712557</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="27">
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="26">
         <v>0.37355732000000003</v>
       </c>
       <c r="C32" s="4">
@@ -1264,10 +1494,14 @@
       <c r="E32" s="4">
         <v>0.43556</v>
       </c>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1287,24 +1521,24 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>5897</v>
@@ -1328,7 +1562,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>318</v>
@@ -1352,7 +1586,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1265</v>
@@ -1376,7 +1610,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>638</v>

</xml_diff>